<commit_message>
[UPDATE] Perubahan format xlsx
</commit_message>
<xml_diff>
--- a/public/docs/sample.xlsx
+++ b/public/docs/sample.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Kategori</t>
   </si>
@@ -35,22 +35,22 @@
     <t>Komoditas (Rp)</t>
   </si>
   <si>
-    <t>Jan  2018</t>
-  </si>
-  <si>
-    <t>Feb  2018</t>
-  </si>
-  <si>
-    <t>Mar  2018</t>
-  </si>
-  <si>
-    <t>Apr  2018</t>
-  </si>
-  <si>
-    <t>Mei  2018</t>
-  </si>
-  <si>
-    <t>Jun  2018</t>
+    <t>1-2018</t>
+  </si>
+  <si>
+    <t>2-2018</t>
+  </si>
+  <si>
+    <t>3-2018</t>
+  </si>
+  <si>
+    <t>4-2018</t>
+  </si>
+  <si>
+    <t>5-2018</t>
+  </si>
+  <si>
+    <t>6-2018</t>
   </si>
   <si>
     <t>Beras</t>
@@ -141,45 +141,6 @@
   </si>
   <si>
     <t>Gula Pasir Lokal</t>
-  </si>
-  <si>
-    <t>Nama Bulan</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>Mei</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Jul</t>
-  </si>
-  <si>
-    <t>Agu</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>Okt</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Des</t>
   </si>
 </sst>
 </file>
@@ -821,9 +782,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1311,7 +1275,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="7"/>
@@ -1333,371 +1297,365 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>10300</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>10450</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>10250</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>10400</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>10300</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>10050</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:8">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>9550</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>9750</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>9600</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>9650</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>9450</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>9300</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" customHeight="1" spans="1:8">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" customHeight="1" spans="1:8">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" customHeight="1" spans="1:8">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" customHeight="1" spans="1:8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" customHeight="1" spans="1:8">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" customHeight="1" spans="1:8">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" customHeight="1" spans="1:8">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" customHeight="1" spans="1:8">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" customHeight="1" spans="1:8">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" customHeight="1" spans="1:8">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" customHeight="1" spans="1:8">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" customHeight="1" spans="1:8">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" customHeight="1" spans="1:8">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" customHeight="1" spans="1:8">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" customHeight="1" spans="1:8">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" customHeight="1" spans="1:8">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" customHeight="1" spans="2:8">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" customHeight="1" spans="1:8">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" customHeight="1" spans="2:8">
       <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1705,78 +1663,58 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" customHeight="1" spans="2:8">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" customHeight="1" spans="2:8">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" customHeight="1" spans="2:3">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" customHeight="1" spans="2:3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" customHeight="1" spans="2:3">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" customHeight="1" spans="2:3">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" customHeight="1" spans="2:3">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" customHeight="1" spans="2:3">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" customHeight="1" spans="2:3">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" customHeight="1" spans="2:3">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" customHeight="1" spans="2:3">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>